<commit_message>
Dont need speed logic
Fuzzy logic is not meant to be perfect and thus the object should be well, more fuzzy on its movement
</commit_message>
<xml_diff>
--- a/AI Project Timetable.xlsx
+++ b/AI Project Timetable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The-w\OneDrive\Documents\Univertsity Year 3 Term 2\MAT301 AI and Mathematics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The-w\OneDrive\Documents\Univertsity Year 3 Term 2\MAT301 AI and Mathematics\Project\MAT301-Unit-1-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1F7C5F-86B4-4AB3-B110-1B8028C9DAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839466F2-8B30-4CC5-AAE4-06745194B971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6EE67C17-ED2E-4F7E-9C97-2292452E076D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Week</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>Speed logic</t>
+  </si>
+  <si>
+    <t>Changing the position of the target</t>
+  </si>
+  <si>
+    <t>Gather data on how it is performing</t>
+  </si>
+  <si>
+    <t>Write the presentation</t>
   </si>
 </sst>
 </file>
@@ -515,7 +524,7 @@
   <dimension ref="A2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,6 +533,9 @@
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -567,6 +579,15 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -588,6 +609,12 @@
       </c>
       <c r="D6" t="s">
         <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Will reset if it doenst find it after 15 seconds
A simple saftey measure in case the random positioning does not work to well.
</commit_message>
<xml_diff>
--- a/AI Project Timetable.xlsx
+++ b/AI Project Timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The-w\OneDrive\Documents\Univertsity Year 3 Term 2\MAT301 AI and Mathematics\Project\MAT301-Unit-1-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839466F2-8B30-4CC5-AAE4-06745194B971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2761F69D-DBFF-447C-986F-08074685FD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6EE67C17-ED2E-4F7E-9C97-2292452E076D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Week</t>
   </si>
@@ -86,13 +86,13 @@
     <t>Speed logic</t>
   </si>
   <si>
-    <t>Changing the position of the target</t>
-  </si>
-  <si>
     <t>Gather data on how it is performing</t>
   </si>
   <si>
-    <t>Write the presentation</t>
+    <t>Write the presentation and record the presentation</t>
+  </si>
+  <si>
+    <t>Changing the position of the target and get the point system working</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,8 +534,8 @@
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="30.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="58.21875" customWidth="1"/>
+    <col min="7" max="7" width="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -568,6 +568,9 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -576,17 +579,17 @@
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -607,14 +610,14 @@
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -623,6 +626,9 @@
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>

</xml_diff>